<commit_message>
Results from July 11, 2020 12:43:08 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -674,13 +674,13 @@
         <v>44023</v>
       </c>
       <c r="C5" t="n">
-        <v>34529</v>
+        <v>34530</v>
       </c>
       <c r="D5" t="n">
         <v>748</v>
       </c>
       <c r="E5" t="n">
-        <v>3000</v>
+        <v>3002</v>
       </c>
       <c r="F5" t="n">
         <v>36</v>
@@ -718,25 +718,25 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C6" t="n">
-        <v>151767</v>
+        <v>152962</v>
       </c>
       <c r="D6" t="n">
-        <v>7144</v>
+        <v>7168</v>
       </c>
       <c r="E6" t="n">
-        <v>25493</v>
+        <v>25689</v>
       </c>
       <c r="F6" t="n">
-        <v>1977</v>
+        <v>1982</v>
       </c>
       <c r="G6" t="n">
-        <v>16.8</v>
+        <v>16.79</v>
       </c>
       <c r="H6" t="n">
-        <v>27.67</v>
+        <v>27.65</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Results from July 11, 2020 12:53:58 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -2165,32 +2165,18 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B36" s="2" t="n">
-        <v>44022</v>
-      </c>
-      <c r="C36" t="n">
-        <v>9928</v>
-      </c>
-      <c r="D36" t="n">
-        <v>101</v>
-      </c>
-      <c r="E36" t="n">
-        <v>145</v>
-      </c>
-      <c r="F36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G36" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.99</v>
-      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
       <c r="I36" t="b">
         <v>0</v>
       </c>
       <c r="J36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2202,7 +2188,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 11, 2020 12:58:09 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -2165,18 +2165,32 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="B36" s="2" t="n">
+        <v>44022</v>
+      </c>
+      <c r="C36" t="n">
+        <v>9928</v>
+      </c>
+      <c r="D36" t="n">
+        <v>101</v>
+      </c>
+      <c r="E36" t="n">
+        <v>145</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.99</v>
+      </c>
       <c r="I36" t="b">
         <v>0</v>
       </c>
       <c r="J36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2188,7 +2202,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 11, 2020 03:03:19 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -573,22 +573,22 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C3" t="n">
-        <v>111110</v>
+        <v>111398</v>
       </c>
       <c r="D3" t="n">
-        <v>8296</v>
+        <v>8310</v>
       </c>
       <c r="E3" t="n">
-        <v>10465</v>
+        <v>10477</v>
       </c>
       <c r="F3" t="n">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="G3" t="n">
-        <v>9.42</v>
+        <v>9.41</v>
       </c>
       <c r="H3" t="n">
         <v>8.23</v>
@@ -674,13 +674,13 @@
         <v>44023</v>
       </c>
       <c r="C5" t="n">
-        <v>34530</v>
+        <v>34647</v>
       </c>
       <c r="D5" t="n">
         <v>748</v>
       </c>
       <c r="E5" t="n">
-        <v>3002</v>
+        <v>3010</v>
       </c>
       <c r="F5" t="n">
         <v>36</v>
@@ -1006,25 +1006,25 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C12" t="n">
-        <v>34753</v>
+        <v>35679</v>
       </c>
       <c r="D12" t="n">
-        <v>814</v>
+        <v>821</v>
       </c>
       <c r="E12" t="n">
-        <v>5845</v>
+        <v>5984</v>
       </c>
       <c r="F12" t="n">
         <v>192</v>
       </c>
       <c r="G12" t="n">
-        <v>18.66</v>
+        <v>18.6</v>
       </c>
       <c r="H12" t="n">
-        <v>23.94</v>
+        <v>23.73</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -1033,10 +1033,10 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>31320</v>
+        <v>32164</v>
       </c>
       <c r="L12" t="n">
-        <v>802</v>
+        <v>809</v>
       </c>
       <c r="M12" t="n">
         <v>368744</v>
@@ -1104,25 +1104,25 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C14" t="n">
-        <v>59546</v>
+        <v>61006</v>
       </c>
       <c r="D14" t="n">
-        <v>723</v>
+        <v>738</v>
       </c>
       <c r="E14" t="n">
-        <v>12100</v>
+        <v>12323</v>
       </c>
       <c r="F14" t="n">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G14" t="n">
-        <v>20.32</v>
+        <v>20.2</v>
       </c>
       <c r="H14" t="n">
-        <v>35.68</v>
+        <v>35.37</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -1206,21 +1206,21 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>28223</t>
+          <t>28855</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>212</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>718</t>
+          <t>731</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1437,22 +1437,22 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C21" t="n">
-        <v>1323</v>
+        <v>1385</v>
       </c>
       <c r="D21" t="n">
         <v>17</v>
       </c>
       <c r="E21" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>1.36</v>
+        <v>1.43</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>2282</v>
+        <v>2376</v>
       </c>
       <c r="L21" t="n">
         <v>34</v>
@@ -2068,25 +2068,25 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C34" t="n">
-        <v>111211</v>
+        <v>114401</v>
       </c>
       <c r="D34" t="n">
-        <v>2965</v>
+        <v>2996</v>
       </c>
       <c r="E34" t="n">
-        <v>30267</v>
+        <v>31052</v>
       </c>
       <c r="F34" t="n">
-        <v>1385</v>
+        <v>1397</v>
       </c>
       <c r="G34" t="n">
-        <v>27.22</v>
+        <v>27.14</v>
       </c>
       <c r="H34" t="n">
-        <v>46.71</v>
+        <v>46.63</v>
       </c>
       <c r="I34" t="b">
         <v>1</v>
@@ -2413,25 +2413,25 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C41" t="n">
-        <v>68207</v>
+        <v>68857</v>
       </c>
       <c r="D41" t="n">
-        <v>5956</v>
+        <v>5983</v>
       </c>
       <c r="E41" t="n">
-        <v>20404</v>
+        <v>20486</v>
       </c>
       <c r="F41" t="n">
-        <v>2375</v>
+        <v>2390</v>
       </c>
       <c r="G41" t="n">
-        <v>29.91</v>
+        <v>29.75</v>
       </c>
       <c r="H41" t="n">
-        <v>39.88</v>
+        <v>39.95</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Results from July 11, 2020 03:06:27 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -2459,32 +2459,18 @@
           <t>Mississippi</t>
         </is>
       </c>
-      <c r="B42" s="2" t="n">
-        <v>44022</v>
-      </c>
-      <c r="C42" t="n">
-        <v>35419</v>
-      </c>
-      <c r="D42" t="n">
-        <v>1230</v>
-      </c>
-      <c r="E42" t="n">
-        <v>16811</v>
-      </c>
-      <c r="F42" t="n">
-        <v>616</v>
-      </c>
-      <c r="G42" t="n">
-        <v>47.46</v>
-      </c>
-      <c r="H42" t="n">
-        <v>50.08</v>
-      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
       <c r="I42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2496,7 +2482,7 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... ConnectionError(ProtocolError('Connection aborted.', ConnectionResetError(104, 'Connection reset by peer')))</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 11, 2020 03:09:47 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -2459,18 +2459,32 @@
           <t>Mississippi</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="B42" s="2" t="n">
+        <v>44022</v>
+      </c>
+      <c r="C42" t="n">
+        <v>35419</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1230</v>
+      </c>
+      <c r="E42" t="n">
+        <v>16811</v>
+      </c>
+      <c r="F42" t="n">
+        <v>616</v>
+      </c>
+      <c r="G42" t="n">
+        <v>47.46</v>
+      </c>
+      <c r="H42" t="n">
+        <v>50.08</v>
+      </c>
       <c r="I42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2482,7 +2496,7 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>An error occurred. ... ConnectionError(ProtocolError('Connection aborted.', ConnectionResetError(104, 'Connection reset by peer')))</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 11, 2020 03:33:27 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -1778,13 +1778,13 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C28" t="n">
-        <v>127358</v>
+        <v>130242</v>
       </c>
       <c r="D28" t="n">
-        <v>3738</v>
+        <v>3793</v>
       </c>
       <c r="E28" t="n">
         <v>3407</v>

</xml_diff>

<commit_message>
Results from July 11, 2020 07:30:40 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -518,47 +518,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C2" t="n">
-        <v>26803</v>
+        <v>25291</v>
       </c>
       <c r="D2" t="n">
-        <v>313</v>
+        <v>717</v>
       </c>
       <c r="E2" t="n">
-        <v>5796</v>
+        <v>2887</v>
       </c>
       <c r="F2" t="n">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G2" t="n">
-        <v>25.01</v>
+        <v>11.42</v>
       </c>
       <c r="H2" t="n">
-        <v>25.26</v>
+        <v>12.69</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>23171</v>
-      </c>
-      <c r="L2" t="n">
-        <v>293</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>460970</v>
+        <v>3365783</v>
       </c>
       <c r="N2" t="n">
-        <v>15.41</v>
+        <v>12.07</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -569,43 +565,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C3" t="n">
-        <v>111398</v>
+        <v>19137</v>
       </c>
       <c r="D3" t="n">
-        <v>8310</v>
+        <v>175</v>
       </c>
       <c r="E3" t="n">
-        <v>10477</v>
+        <v>464</v>
       </c>
       <c r="F3" t="n">
-        <v>684</v>
+        <v>17</v>
       </c>
       <c r="G3" t="n">
-        <v>9.41</v>
+        <v>6.81</v>
       </c>
       <c r="H3" t="n">
-        <v>8.23</v>
+        <v>15.32</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>6812</v>
+      </c>
+      <c r="L3" t="n">
+        <v>111</v>
+      </c>
       <c r="M3" t="n">
-        <v>510558</v>
+        <v>146703</v>
       </c>
       <c r="N3" t="n">
-        <v>7.48</v>
+        <v>7.62</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -616,47 +616,51 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>New York -- New York</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
         <v>44023</v>
       </c>
-      <c r="C4" t="n">
-        <v>51294</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1086</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>215598</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18667</t>
+        </is>
       </c>
       <c r="E4" t="n">
-        <v>17111</v>
+        <v>33453</v>
       </c>
       <c r="F4" t="n">
-        <v>479</v>
+        <v>5225</v>
       </c>
       <c r="G4" t="n">
-        <v>45.22</v>
+        <v>30.15</v>
       </c>
       <c r="H4" t="n">
-        <v>45.84</v>
+        <v>30.52</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>37836</v>
+        <v>110942</v>
       </c>
       <c r="L4" t="n">
-        <v>1045</v>
+        <v>17118</v>
       </c>
       <c r="M4" t="n">
-        <v>1293186</v>
+        <v>2049418</v>
       </c>
       <c r="N4" t="n">
-        <v>26.58</v>
+        <v>24.27</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -667,43 +671,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44023</v>
+        <v>44015</v>
       </c>
       <c r="C5" t="n">
-        <v>34647</v>
+        <v>16491</v>
       </c>
       <c r="D5" t="n">
-        <v>748</v>
+        <v>960</v>
       </c>
       <c r="E5" t="n">
-        <v>3010</v>
+        <v>1592</v>
       </c>
       <c r="F5" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G5" t="n">
-        <v>8.69</v>
+        <v>12.29</v>
       </c>
       <c r="H5" t="n">
-        <v>4.81</v>
+        <v>6.14</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>12950</v>
+      </c>
+      <c r="L5" t="n">
+        <v>782</v>
+      </c>
       <c r="M5" t="n">
-        <v>109911</v>
+        <v>69254</v>
       </c>
       <c r="N5" t="n">
-        <v>3.51</v>
+        <v>6.55</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -714,43 +722,43 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C6" t="n">
-        <v>152962</v>
+        <v>61006</v>
       </c>
       <c r="D6" t="n">
-        <v>7168</v>
+        <v>738</v>
       </c>
       <c r="E6" t="n">
-        <v>25689</v>
+        <v>12323</v>
       </c>
       <c r="F6" t="n">
-        <v>1982</v>
+        <v>261</v>
       </c>
       <c r="G6" t="n">
-        <v>16.79</v>
+        <v>20.2</v>
       </c>
       <c r="H6" t="n">
-        <v>27.65</v>
+        <v>35.37</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>1824125</v>
+        <v>1117489</v>
       </c>
       <c r="N6" t="n">
-        <v>14.23</v>
+        <v>16.8</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -761,41 +769,49 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
         <v>44023</v>
       </c>
-      <c r="C7" t="n">
-        <v>3520</v>
-      </c>
-      <c r="D7" t="n">
-        <v>112</v>
-      </c>
-      <c r="E7" t="n">
-        <v>814</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>28855</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>731</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>&lt;5</t>
+        </is>
+      </c>
       <c r="G7" t="n">
-        <v>25.94</v>
+        <v>2.5</v>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3138</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>17881</v>
+        <v>35862</v>
       </c>
       <c r="N7" t="n">
-        <v>1.34</v>
+        <v>1.18</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -806,47 +822,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C8" t="n">
-        <v>18602</v>
+        <v>19121</v>
       </c>
       <c r="D8" t="n">
-        <v>166</v>
+        <v>622</v>
       </c>
       <c r="E8" t="n">
-        <v>464</v>
+        <v>2091</v>
       </c>
       <c r="F8" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G8" t="n">
-        <v>6.81</v>
+        <v>16.08</v>
       </c>
       <c r="H8" t="n">
-        <v>15.32</v>
+        <v>4.14</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>6812</v>
+        <v>13008</v>
       </c>
       <c r="L8" t="n">
-        <v>111</v>
+        <v>583</v>
       </c>
       <c r="M8" t="n">
-        <v>146703</v>
+        <v>354112</v>
       </c>
       <c r="N8" t="n">
-        <v>7.62</v>
+        <v>7.98</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -857,43 +873,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44021</v>
+        <v>44023</v>
       </c>
       <c r="C9" t="n">
-        <v>10679</v>
+        <v>27864</v>
       </c>
       <c r="D9" t="n">
-        <v>568</v>
+        <v>319</v>
       </c>
       <c r="E9" t="n">
-        <v>5266</v>
+        <v>5959</v>
       </c>
       <c r="F9" t="n">
-        <v>421</v>
+        <v>77</v>
       </c>
       <c r="G9" t="n">
-        <v>49.31</v>
+        <v>24.83</v>
       </c>
       <c r="H9" t="n">
-        <v>74.12</v>
+        <v>25.84</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>24000</v>
+      </c>
+      <c r="L9" t="n">
+        <v>298</v>
+      </c>
       <c r="M9" t="n">
-        <v>321317</v>
+        <v>460970</v>
       </c>
       <c r="N9" t="n">
-        <v>46.94</v>
+        <v>15.41</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -904,47 +924,47 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>California - San Diego</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C10" t="n">
-        <v>18670</v>
+        <v>19371</v>
       </c>
       <c r="D10" t="n">
-        <v>620</v>
+        <v>422</v>
       </c>
       <c r="E10" t="n">
-        <v>1756</v>
+        <v>712</v>
       </c>
       <c r="F10" t="n">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="G10" t="n">
-        <v>13.57</v>
+        <v>4.61</v>
       </c>
       <c r="H10" t="n">
-        <v>15.29</v>
+        <v>3.87</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>12943</v>
+        <v>15451</v>
       </c>
       <c r="L10" t="n">
-        <v>581</v>
+        <v>413</v>
       </c>
       <c r="M10" t="n">
-        <v>354112</v>
+        <v>166412</v>
       </c>
       <c r="N10" t="n">
-        <v>7.98</v>
+        <v>5.04</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -955,29 +975,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C11" t="n">
-        <v>41571</v>
+        <v>69782</v>
       </c>
       <c r="D11" t="n">
-        <v>1499</v>
+        <v>1962</v>
       </c>
       <c r="E11" t="n">
-        <v>8571</v>
+        <v>10606</v>
       </c>
       <c r="F11" t="n">
-        <v>147</v>
+        <v>456</v>
       </c>
       <c r="G11" t="n">
-        <v>20.62</v>
+        <v>15.2</v>
       </c>
       <c r="H11" t="n">
-        <v>9.81</v>
+        <v>23.24</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -988,10 +1008,10 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>342186</v>
+        <v>1613285</v>
       </c>
       <c r="N11" t="n">
-        <v>6.19</v>
+        <v>19.17</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1002,47 +1022,39 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C12" t="n">
-        <v>35679</v>
+        <v>14773</v>
       </c>
       <c r="D12" t="n">
-        <v>821</v>
+        <v>543</v>
       </c>
       <c r="E12" t="n">
-        <v>5984</v>
-      </c>
-      <c r="F12" t="n">
-        <v>192</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>18.6</v>
-      </c>
-      <c r="H12" t="n">
-        <v>23.73</v>
-      </c>
+        <v>1.89</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="n">
-        <v>32164</v>
-      </c>
-      <c r="L12" t="n">
-        <v>809</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>368744</v>
+        <v>43006</v>
       </c>
       <c r="N12" t="n">
-        <v>6.38</v>
+        <v>2.06</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1053,43 +1065,41 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Florida -- Miami-Dade County</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C13" t="n">
-        <v>51079</v>
+        <v>60868</v>
       </c>
       <c r="D13" t="n">
-        <v>2563</v>
+        <v>1132</v>
       </c>
       <c r="E13" t="n">
-        <v>6064</v>
-      </c>
-      <c r="F13" t="n">
-        <v>370</v>
-      </c>
+        <v>6886</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="H13" t="n">
-        <v>14.44</v>
-      </c>
+        <v>20.53</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>33549</v>
+      </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>619472</v>
+        <v>481976</v>
       </c>
       <c r="N13" t="n">
-        <v>9.33</v>
+        <v>17.75</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1100,43 +1110,41 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Florida -- Orange County</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C14" t="n">
-        <v>61006</v>
+        <v>16630</v>
       </c>
       <c r="D14" t="n">
-        <v>738</v>
+        <v>80</v>
       </c>
       <c r="E14" t="n">
-        <v>12323</v>
-      </c>
-      <c r="F14" t="n">
-        <v>261</v>
-      </c>
+        <v>2220</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="H14" t="n">
-        <v>35.37</v>
-      </c>
+        <v>24.57</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>9034</v>
+      </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>1117489</v>
+        <v>277193</v>
       </c>
       <c r="N14" t="n">
-        <v>16.8</v>
+        <v>20.98</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1147,51 +1155,47 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
         <v>44023</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215598</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>18667</t>
-        </is>
+      <c r="C15" t="n">
+        <v>51294</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1086</v>
       </c>
       <c r="E15" t="n">
-        <v>33453</v>
+        <v>17111</v>
       </c>
       <c r="F15" t="n">
-        <v>5225</v>
+        <v>479</v>
       </c>
       <c r="G15" t="n">
-        <v>30.15</v>
+        <v>45.22</v>
       </c>
       <c r="H15" t="n">
-        <v>30.52</v>
+        <v>45.84</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>110942</v>
+        <v>37836</v>
       </c>
       <c r="L15" t="n">
-        <v>17118</v>
+        <v>1045</v>
       </c>
       <c r="M15" t="n">
-        <v>2049418</v>
+        <v>1293186</v>
       </c>
       <c r="N15" t="n">
-        <v>24.27</v>
+        <v>26.58</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1202,49 +1206,47 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>California - Los Angeles</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44023</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>28855</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>212</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>731</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>&lt;5</t>
-        </is>
+        <v>44022</v>
+      </c>
+      <c r="C16" t="n">
+        <v>130242</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3793</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3476</v>
+      </c>
+      <c r="F16" t="n">
+        <v>386</v>
       </c>
       <c r="G16" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H16" t="inlineStr"/>
+        <v>4.74</v>
+      </c>
+      <c r="H16" t="n">
+        <v>10.94</v>
+      </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>73398</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3529</v>
+      </c>
       <c r="M16" t="n">
-        <v>35862</v>
+        <v>823987</v>
       </c>
       <c r="N16" t="n">
-        <v>1.18</v>
+        <v>8.16</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1255,47 +1257,47 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Vermont</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C17" t="n">
-        <v>1283</v>
+        <v>72467</v>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>3179</v>
       </c>
       <c r="E17" t="n">
-        <v>138</v>
+        <v>20910</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1289</v>
       </c>
       <c r="G17" t="n">
-        <v>11.05</v>
+        <v>28.85</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>40.55</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>1249</v>
+        <v>59766</v>
       </c>
       <c r="L17" t="n">
-        <v>56</v>
+        <v>72448</v>
       </c>
       <c r="M17" t="n">
-        <v>8058</v>
+        <v>1788090</v>
       </c>
       <c r="N17" t="n">
-        <v>1.29</v>
+        <v>29.78</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1306,47 +1308,43 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44009</v>
+        <v>44022</v>
       </c>
       <c r="C18" t="n">
-        <v>20261</v>
+        <v>35419</v>
       </c>
       <c r="D18" t="n">
-        <v>996</v>
+        <v>1230</v>
       </c>
       <c r="E18" t="n">
-        <v>5758</v>
+        <v>16811</v>
       </c>
       <c r="F18" t="n">
-        <v>246</v>
+        <v>616</v>
       </c>
       <c r="G18" t="n">
-        <v>49.66</v>
+        <v>47.46</v>
       </c>
       <c r="H18" t="n">
-        <v>38.56</v>
+        <v>50.08</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
       </c>
-      <c r="K18" t="n">
-        <v>11594</v>
-      </c>
-      <c r="L18" t="n">
-        <v>638</v>
-      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>704896</v>
+        <v>1125834</v>
       </c>
       <c r="N18" t="n">
-        <v>11.57</v>
+        <v>37.67</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1357,59 +1355,81 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>California</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+          <t>Pennsylvania</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44023</v>
+      </c>
+      <c r="C19" t="n">
+        <v>92001</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6897</v>
+      </c>
+      <c r="E19" t="n">
+        <v>12624</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1426</v>
+      </c>
+      <c r="G19" t="n">
+        <v>30.31</v>
+      </c>
+      <c r="H19" t="n">
+        <v>21.68</v>
+      </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>41651</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6579</v>
+      </c>
       <c r="M19" t="n">
-        <v>2267875</v>
+        <v>1423319</v>
       </c>
       <c r="N19" t="n">
-        <v>5.79</v>
+        <v>11.13</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C20" t="n">
-        <v>14549</v>
+        <v>250984</v>
       </c>
       <c r="D20" t="n">
-        <v>539</v>
+        <v>4197</v>
       </c>
       <c r="E20" t="n">
-        <v>277</v>
-      </c>
-      <c r="F20" t="inlineStr"/>
+        <v>32370</v>
+      </c>
+      <c r="F20" t="n">
+        <v>821</v>
+      </c>
       <c r="G20" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="H20" t="inlineStr"/>
+        <v>12.9</v>
+      </c>
+      <c r="H20" t="n">
+        <v>19.56</v>
+      </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
@@ -1419,10 +1439,10 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>43006</v>
+        <v>3316376</v>
       </c>
       <c r="N20" t="n">
-        <v>2.06</v>
+        <v>16.1</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1433,47 +1453,39 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C21" t="n">
-        <v>1385</v>
+        <v>1677</v>
       </c>
       <c r="D21" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E21" t="n">
-        <v>34</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
+        <v>0.42</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
       </c>
-      <c r="K21" t="n">
-        <v>2376</v>
-      </c>
-      <c r="L21" t="n">
-        <v>34</v>
-      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>24129</v>
+        <v>4630</v>
       </c>
       <c r="N21" t="n">
-        <v>3.27</v>
+        <v>0.44</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1484,43 +1496,47 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C22" t="n">
-        <v>24758</v>
+        <v>1283</v>
       </c>
       <c r="D22" t="n">
-        <v>710</v>
+        <v>56</v>
       </c>
       <c r="E22" t="n">
-        <v>2851</v>
+        <v>138</v>
       </c>
       <c r="F22" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>11.52</v>
+        <v>11.05</v>
       </c>
       <c r="H22" t="n">
-        <v>12.82</v>
+        <v>0</v>
       </c>
       <c r="I22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1249</v>
+      </c>
+      <c r="L22" t="n">
+        <v>56</v>
+      </c>
       <c r="M22" t="n">
-        <v>3365783</v>
+        <v>8058</v>
       </c>
       <c r="N22" t="n">
-        <v>12.07</v>
+        <v>1.29</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1531,47 +1547,43 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44023</v>
+        <v>44021</v>
       </c>
       <c r="C23" t="n">
-        <v>72467</v>
+        <v>45308</v>
       </c>
       <c r="D23" t="n">
-        <v>3179</v>
+        <v>3476</v>
       </c>
       <c r="E23" t="n">
-        <v>20910</v>
+        <v>6189</v>
       </c>
       <c r="F23" t="n">
-        <v>1289</v>
+        <v>646</v>
       </c>
       <c r="G23" t="n">
-        <v>28.85</v>
+        <v>13.66</v>
       </c>
       <c r="H23" t="n">
-        <v>40.55</v>
+        <v>18.58</v>
       </c>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
       </c>
-      <c r="K23" t="n">
-        <v>59766</v>
-      </c>
-      <c r="L23" t="n">
-        <v>72448</v>
-      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>1788090</v>
+        <v>378262</v>
       </c>
       <c r="N23" t="n">
-        <v>29.78</v>
+        <v>10.56</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1582,29 +1594,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C24" t="n">
-        <v>18863</v>
+        <v>36591</v>
       </c>
       <c r="D24" t="n">
-        <v>420</v>
+        <v>1725</v>
       </c>
       <c r="E24" t="n">
-        <v>690</v>
+        <v>1881</v>
       </c>
       <c r="F24" t="n">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="G24" t="n">
-        <v>4.58</v>
+        <v>6.34</v>
       </c>
       <c r="H24" t="n">
-        <v>3.89</v>
+        <v>7.04</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
@@ -1613,16 +1625,16 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>15058</v>
+        <v>29686</v>
       </c>
       <c r="L24" t="n">
-        <v>411</v>
+        <v>1662</v>
       </c>
       <c r="M24" t="n">
-        <v>166412</v>
+        <v>227938</v>
       </c>
       <c r="N24" t="n">
-        <v>5.04</v>
+        <v>4.12</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1633,26 +1645,30 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Florida -- Miami-Dade County</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C25" t="n">
-        <v>60868</v>
+        <v>20998</v>
       </c>
       <c r="D25" t="n">
-        <v>1132</v>
+        <v>285</v>
       </c>
       <c r="E25" t="n">
-        <v>6886</v>
-      </c>
-      <c r="F25" t="inlineStr"/>
+        <v>1230</v>
+      </c>
+      <c r="F25" t="n">
+        <v>22</v>
+      </c>
       <c r="G25" t="n">
-        <v>20.53</v>
-      </c>
-      <c r="H25" t="inlineStr"/>
+        <v>7.61</v>
+      </c>
+      <c r="H25" t="n">
+        <v>8.029999999999999</v>
+      </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
@@ -1660,14 +1676,16 @@
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>33549</v>
-      </c>
-      <c r="L25" t="inlineStr"/>
+        <v>16169</v>
+      </c>
+      <c r="L25" t="n">
+        <v>274</v>
+      </c>
       <c r="M25" t="n">
-        <v>481976</v>
+        <v>90860</v>
       </c>
       <c r="N25" t="n">
-        <v>17.75</v>
+        <v>4.77</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -1678,41 +1696,43 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Florida -- Orange County</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C26" t="n">
-        <v>16630</v>
+        <v>68857</v>
       </c>
       <c r="D26" t="n">
-        <v>80</v>
+        <v>5983</v>
       </c>
       <c r="E26" t="n">
-        <v>2220</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
+        <v>20486</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2390</v>
+      </c>
       <c r="G26" t="n">
-        <v>24.57</v>
-      </c>
-      <c r="H26" t="inlineStr"/>
+        <v>29.75</v>
+      </c>
+      <c r="H26" t="n">
+        <v>39.95</v>
+      </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26" t="n">
-        <v>9034</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
-        <v>277193</v>
+        <v>1375424</v>
       </c>
       <c r="N26" t="n">
-        <v>20.98</v>
+        <v>13.81</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1723,98 +1743,76 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>North Carolina</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>44023</v>
-      </c>
-      <c r="C27" t="n">
-        <v>83793</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1499</v>
-      </c>
-      <c r="E27" t="n">
-        <v>13702</v>
-      </c>
-      <c r="F27" t="n">
-        <v>474</v>
-      </c>
-      <c r="G27" t="n">
-        <v>23.88</v>
-      </c>
-      <c r="H27" t="n">
-        <v>32.8</v>
-      </c>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
-      </c>
-      <c r="K27" t="n">
-        <v>57384</v>
-      </c>
-      <c r="L27" t="n">
-        <v>1445</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="n">
-        <v>2179622</v>
+        <v>2267875</v>
       </c>
       <c r="N27" t="n">
-        <v>21.46</v>
+        <v>5.79</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C28" t="n">
-        <v>130242</v>
+        <v>51079</v>
       </c>
       <c r="D28" t="n">
-        <v>3793</v>
+        <v>2563</v>
       </c>
       <c r="E28" t="n">
-        <v>3407</v>
+        <v>6064</v>
       </c>
       <c r="F28" t="n">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="G28" t="n">
-        <v>4.76</v>
+        <v>11.87</v>
       </c>
       <c r="H28" t="n">
-        <v>10.91</v>
+        <v>14.44</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>71628</v>
-      </c>
-      <c r="L28" t="n">
-        <v>3482</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>823987</v>
+        <v>619472</v>
       </c>
       <c r="N28" t="n">
-        <v>8.16</v>
+        <v>9.33</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1825,39 +1823,47 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C29" t="n">
-        <v>1677</v>
+        <v>1385</v>
       </c>
       <c r="D29" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
-      </c>
-      <c r="F29" t="inlineStr"/>
+        <v>34</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
       <c r="G29" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="H29" t="inlineStr"/>
+        <v>1.43</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="b">
         <v>1</v>
       </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
+      <c r="K29" t="n">
+        <v>2376</v>
+      </c>
+      <c r="L29" t="n">
+        <v>34</v>
+      </c>
       <c r="M29" t="n">
-        <v>4630</v>
+        <v>24129</v>
       </c>
       <c r="N29" t="n">
-        <v>0.44</v>
+        <v>3.27</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1868,43 +1874,47 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Connecticut</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44021</v>
+        <v>44023</v>
       </c>
       <c r="C30" t="n">
-        <v>45308</v>
+        <v>35679</v>
       </c>
       <c r="D30" t="n">
-        <v>3476</v>
+        <v>821</v>
       </c>
       <c r="E30" t="n">
-        <v>6189</v>
+        <v>5984</v>
       </c>
       <c r="F30" t="n">
-        <v>646</v>
+        <v>192</v>
       </c>
       <c r="G30" t="n">
-        <v>13.66</v>
+        <v>18.6</v>
       </c>
       <c r="H30" t="n">
-        <v>18.58</v>
+        <v>23.73</v>
       </c>
       <c r="I30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K30" t="n">
+        <v>32164</v>
+      </c>
+      <c r="L30" t="n">
+        <v>809</v>
+      </c>
       <c r="M30" t="n">
-        <v>378262</v>
+        <v>368744</v>
       </c>
       <c r="N30" t="n">
-        <v>10.56</v>
+        <v>6.38</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1915,29 +1925,29 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C31" t="n">
-        <v>69782</v>
+        <v>114401</v>
       </c>
       <c r="D31" t="n">
-        <v>1962</v>
+        <v>2996</v>
       </c>
       <c r="E31" t="n">
-        <v>10606</v>
+        <v>31052</v>
       </c>
       <c r="F31" t="n">
-        <v>456</v>
+        <v>1397</v>
       </c>
       <c r="G31" t="n">
-        <v>15.2</v>
+        <v>27.14</v>
       </c>
       <c r="H31" t="n">
-        <v>23.24</v>
+        <v>46.63</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -1948,10 +1958,10 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="n">
-        <v>1613285</v>
+        <v>3239300</v>
       </c>
       <c r="N31" t="n">
-        <v>19.17</v>
+        <v>31.46</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -1962,29 +1972,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44015</v>
+        <v>44022</v>
       </c>
       <c r="C32" t="n">
-        <v>16491</v>
+        <v>39218</v>
       </c>
       <c r="D32" t="n">
-        <v>960</v>
+        <v>1424</v>
       </c>
       <c r="E32" t="n">
-        <v>1592</v>
+        <v>1520</v>
       </c>
       <c r="F32" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G32" t="n">
-        <v>12.29</v>
+        <v>5.43</v>
       </c>
       <c r="H32" t="n">
-        <v>6.14</v>
+        <v>3.39</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -1993,16 +2003,16 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>12950</v>
+        <v>27979</v>
       </c>
       <c r="L32" t="n">
-        <v>782</v>
+        <v>1355</v>
       </c>
       <c r="M32" t="n">
-        <v>69254</v>
+        <v>269854</v>
       </c>
       <c r="N32" t="n">
-        <v>6.55</v>
+        <v>3.7</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2013,47 +2023,43 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44022</v>
+        <v>44021</v>
       </c>
       <c r="C33" t="n">
-        <v>20777</v>
+        <v>10679</v>
       </c>
       <c r="D33" t="n">
-        <v>286</v>
+        <v>568</v>
       </c>
       <c r="E33" t="n">
-        <v>1230</v>
+        <v>5266</v>
       </c>
       <c r="F33" t="n">
-        <v>22</v>
+        <v>421</v>
       </c>
       <c r="G33" t="n">
-        <v>7.61</v>
+        <v>49.31</v>
       </c>
       <c r="H33" t="n">
-        <v>8.029999999999999</v>
+        <v>74.12</v>
       </c>
       <c r="I33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="b">
         <v>1</v>
       </c>
-      <c r="K33" t="n">
-        <v>16169</v>
-      </c>
-      <c r="L33" t="n">
-        <v>274</v>
-      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
       <c r="M33" t="n">
-        <v>90860</v>
+        <v>321317</v>
       </c>
       <c r="N33" t="n">
-        <v>4.77</v>
+        <v>46.94</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2064,43 +2070,43 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C34" t="n">
-        <v>114401</v>
+        <v>12743</v>
       </c>
       <c r="D34" t="n">
-        <v>2996</v>
+        <v>106</v>
       </c>
       <c r="E34" t="n">
-        <v>31052</v>
+        <v>3254</v>
       </c>
       <c r="F34" t="n">
-        <v>1397</v>
+        <v>132</v>
       </c>
       <c r="G34" t="n">
-        <v>27.14</v>
+        <v>25.54</v>
       </c>
       <c r="H34" t="n">
-        <v>46.63</v>
+        <v>124.53</v>
       </c>
       <c r="I34" t="b">
         <v>1</v>
       </c>
       <c r="J34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>3239300</v>
+        <v>209892</v>
       </c>
       <c r="N34" t="n">
-        <v>31.46</v>
+        <v>22.11</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2111,47 +2117,41 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C35" t="n">
-        <v>13430</v>
+        <v>3520</v>
       </c>
       <c r="D35" t="n">
-        <v>359</v>
+        <v>112</v>
       </c>
       <c r="E35" t="n">
-        <v>3889</v>
-      </c>
-      <c r="F35" t="n">
-        <v>145</v>
-      </c>
+        <v>814</v>
+      </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
-        <v>31.17</v>
-      </c>
-      <c r="H35" t="n">
-        <v>40.39</v>
-      </c>
+        <v>25.94</v>
+      </c>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>12475</v>
-      </c>
-      <c r="L35" t="n">
-        <v>359</v>
-      </c>
+        <v>3138</v>
+      </c>
+      <c r="L35" t="inlineStr"/>
       <c r="M35" t="n">
-        <v>252321</v>
+        <v>17881</v>
       </c>
       <c r="N35" t="n">
-        <v>26.44</v>
+        <v>1.34</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2162,32 +2162,32 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Idaho</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C36" t="n">
-        <v>9928</v>
+        <v>34658</v>
       </c>
       <c r="D36" t="n">
-        <v>101</v>
+        <v>748</v>
       </c>
       <c r="E36" t="n">
-        <v>145</v>
+        <v>3011</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="G36" t="n">
-        <v>1.46</v>
+        <v>8.69</v>
       </c>
       <c r="H36" t="n">
-        <v>0.99</v>
+        <v>4.81</v>
       </c>
       <c r="I36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>
@@ -2195,10 +2195,10 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
-        <v>11536</v>
+        <v>109911</v>
       </c>
       <c r="N36" t="n">
-        <v>0.68</v>
+        <v>3.51</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2209,29 +2209,29 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C37" t="n">
-        <v>92001</v>
+        <v>83793</v>
       </c>
       <c r="D37" t="n">
-        <v>6897</v>
+        <v>1499</v>
       </c>
       <c r="E37" t="n">
-        <v>12624</v>
+        <v>13702</v>
       </c>
       <c r="F37" t="n">
-        <v>1426</v>
+        <v>474</v>
       </c>
       <c r="G37" t="n">
-        <v>30.31</v>
+        <v>23.88</v>
       </c>
       <c r="H37" t="n">
-        <v>21.68</v>
+        <v>32.8</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -2240,16 +2240,16 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>41651</v>
+        <v>57384</v>
       </c>
       <c r="L37" t="n">
-        <v>6579</v>
+        <v>1445</v>
       </c>
       <c r="M37" t="n">
-        <v>1423319</v>
+        <v>2179622</v>
       </c>
       <c r="N37" t="n">
-        <v>11.13</v>
+        <v>21.46</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2260,47 +2260,43 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C38" t="n">
-        <v>36191</v>
+        <v>152962</v>
       </c>
       <c r="D38" t="n">
-        <v>1724</v>
+        <v>7168</v>
       </c>
       <c r="E38" t="n">
-        <v>1871</v>
+        <v>25689</v>
       </c>
       <c r="F38" t="n">
-        <v>117</v>
+        <v>1982</v>
       </c>
       <c r="G38" t="n">
-        <v>6.35</v>
+        <v>16.79</v>
       </c>
       <c r="H38" t="n">
-        <v>7.04</v>
+        <v>27.65</v>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
       </c>
-      <c r="K38" t="n">
-        <v>29452</v>
-      </c>
-      <c r="L38" t="n">
-        <v>1661</v>
-      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
       <c r="M38" t="n">
-        <v>227938</v>
+        <v>1824125</v>
       </c>
       <c r="N38" t="n">
-        <v>4.12</v>
+        <v>14.23</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2311,47 +2307,43 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="C39" t="n">
-        <v>39218</v>
+        <v>10505</v>
       </c>
       <c r="D39" t="n">
-        <v>1424</v>
+        <v>101</v>
       </c>
       <c r="E39" t="n">
-        <v>1520</v>
+        <v>149</v>
       </c>
       <c r="F39" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>5.43</v>
+        <v>1.42</v>
       </c>
       <c r="H39" t="n">
-        <v>3.39</v>
+        <v>0.99</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="b">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
-        <v>27979</v>
-      </c>
-      <c r="L39" t="n">
-        <v>1355</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
       <c r="M39" t="n">
-        <v>269854</v>
+        <v>11536</v>
       </c>
       <c r="N39" t="n">
-        <v>3.7</v>
+        <v>0.68</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -2362,43 +2354,43 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C40" t="n">
-        <v>250984</v>
+        <v>41571</v>
       </c>
       <c r="D40" t="n">
-        <v>4197</v>
+        <v>1499</v>
       </c>
       <c r="E40" t="n">
-        <v>32370</v>
+        <v>8571</v>
       </c>
       <c r="F40" t="n">
-        <v>821</v>
+        <v>147</v>
       </c>
       <c r="G40" t="n">
-        <v>12.9</v>
+        <v>20.62</v>
       </c>
       <c r="H40" t="n">
-        <v>19.56</v>
+        <v>9.81</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="n">
-        <v>3316376</v>
+        <v>342186</v>
       </c>
       <c r="N40" t="n">
-        <v>16.1</v>
+        <v>6.19</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2409,29 +2401,29 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C41" t="n">
-        <v>68857</v>
+        <v>111398</v>
       </c>
       <c r="D41" t="n">
-        <v>5983</v>
+        <v>8310</v>
       </c>
       <c r="E41" t="n">
-        <v>20486</v>
+        <v>10477</v>
       </c>
       <c r="F41" t="n">
-        <v>2390</v>
+        <v>684</v>
       </c>
       <c r="G41" t="n">
-        <v>29.75</v>
+        <v>9.41</v>
       </c>
       <c r="H41" t="n">
-        <v>39.95</v>
+        <v>8.23</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
@@ -2442,10 +2434,10 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="n">
-        <v>1375424</v>
+        <v>510558</v>
       </c>
       <c r="N41" t="n">
-        <v>13.81</v>
+        <v>7.48</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -2456,43 +2448,47 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mississippi</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
         <v>44022</v>
       </c>
       <c r="C42" t="n">
-        <v>35419</v>
+        <v>13430</v>
       </c>
       <c r="D42" t="n">
-        <v>1230</v>
+        <v>359</v>
       </c>
       <c r="E42" t="n">
-        <v>16811</v>
+        <v>3889</v>
       </c>
       <c r="F42" t="n">
-        <v>616</v>
+        <v>145</v>
       </c>
       <c r="G42" t="n">
-        <v>47.46</v>
+        <v>31.17</v>
       </c>
       <c r="H42" t="n">
-        <v>50.08</v>
+        <v>40.39</v>
       </c>
       <c r="I42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="b">
-        <v>1</v>
-      </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>12475</v>
+      </c>
+      <c r="L42" t="n">
+        <v>359</v>
+      </c>
       <c r="M42" t="n">
-        <v>1125834</v>
+        <v>252321</v>
       </c>
       <c r="N42" t="n">
-        <v>37.67</v>
+        <v>26.44</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -2503,43 +2499,47 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44023</v>
+        <v>44009</v>
       </c>
       <c r="C43" t="n">
-        <v>12743</v>
+        <v>20261</v>
       </c>
       <c r="D43" t="n">
-        <v>106</v>
+        <v>996</v>
       </c>
       <c r="E43" t="n">
-        <v>3254</v>
+        <v>5758</v>
       </c>
       <c r="F43" t="n">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="G43" t="n">
-        <v>25.54</v>
+        <v>49.66</v>
       </c>
       <c r="H43" t="n">
-        <v>124.53</v>
+        <v>38.56</v>
       </c>
       <c r="I43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
-      </c>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K43" t="n">
+        <v>11594</v>
+      </c>
+      <c r="L43" t="n">
+        <v>638</v>
+      </c>
       <c r="M43" t="n">
-        <v>209892</v>
+        <v>704896</v>
       </c>
       <c r="N43" t="n">
-        <v>22.11</v>
+        <v>11.57</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Results from July 11, 2020 11:49:36 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-11.xlsx
@@ -518,43 +518,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C2" t="n">
-        <v>25291</v>
+        <v>27864</v>
       </c>
       <c r="D2" t="n">
-        <v>717</v>
+        <v>319</v>
       </c>
       <c r="E2" t="n">
-        <v>2887</v>
+        <v>5959</v>
       </c>
       <c r="F2" t="n">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G2" t="n">
-        <v>11.42</v>
+        <v>24.83</v>
       </c>
       <c r="H2" t="n">
-        <v>12.69</v>
+        <v>25.84</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>24000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>298</v>
+      </c>
       <c r="M2" t="n">
-        <v>3365783</v>
+        <v>460970</v>
       </c>
       <c r="N2" t="n">
-        <v>12.07</v>
+        <v>15.41</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -565,47 +569,43 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C3" t="n">
-        <v>19137</v>
+        <v>111398</v>
       </c>
       <c r="D3" t="n">
-        <v>175</v>
+        <v>8310</v>
       </c>
       <c r="E3" t="n">
-        <v>464</v>
+        <v>10477</v>
       </c>
       <c r="F3" t="n">
-        <v>17</v>
+        <v>684</v>
       </c>
       <c r="G3" t="n">
-        <v>6.81</v>
+        <v>9.41</v>
       </c>
       <c r="H3" t="n">
-        <v>15.32</v>
+        <v>8.23</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="n">
-        <v>6812</v>
-      </c>
-      <c r="L3" t="n">
-        <v>111</v>
-      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>146703</v>
+        <v>510558</v>
       </c>
       <c r="N3" t="n">
-        <v>7.62</v>
+        <v>7.48</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -616,102 +616,76 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>44023</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>215598</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18667</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>33453</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5225</v>
-      </c>
-      <c r="G4" t="n">
-        <v>30.15</v>
-      </c>
-      <c r="H4" t="n">
-        <v>30.52</v>
-      </c>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>110942</v>
-      </c>
-      <c r="L4" t="n">
-        <v>17118</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
-        <v>2049418</v>
+        <v>1293186</v>
       </c>
       <c r="N4" t="n">
-        <v>24.27</v>
+        <v>26.58</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... Exception('Your request has timed out.\n(Error Code: 504)')</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44015</v>
+        <v>44023</v>
       </c>
       <c r="C5" t="n">
-        <v>16491</v>
+        <v>34695</v>
       </c>
       <c r="D5" t="n">
-        <v>960</v>
+        <v>748</v>
       </c>
       <c r="E5" t="n">
-        <v>1592</v>
+        <v>3011</v>
       </c>
       <c r="F5" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G5" t="n">
-        <v>12.29</v>
+        <v>8.68</v>
       </c>
       <c r="H5" t="n">
-        <v>6.14</v>
+        <v>4.81</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>12950</v>
-      </c>
-      <c r="L5" t="n">
-        <v>782</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>69254</v>
+        <v>109911</v>
       </c>
       <c r="N5" t="n">
-        <v>6.55</v>
+        <v>3.51</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -722,43 +696,43 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C6" t="n">
-        <v>61006</v>
+        <v>152962</v>
       </c>
       <c r="D6" t="n">
-        <v>738</v>
+        <v>7168</v>
       </c>
       <c r="E6" t="n">
-        <v>12323</v>
+        <v>25689</v>
       </c>
       <c r="F6" t="n">
-        <v>261</v>
+        <v>1982</v>
       </c>
       <c r="G6" t="n">
-        <v>20.2</v>
+        <v>16.79</v>
       </c>
       <c r="H6" t="n">
-        <v>35.37</v>
+        <v>27.65</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
       <c r="J6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>1117489</v>
+        <v>1824125</v>
       </c>
       <c r="N6" t="n">
-        <v>16.8</v>
+        <v>14.23</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -769,49 +743,41 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
         <v>44023</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>28855</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>212</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>731</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>&lt;5</t>
-        </is>
-      </c>
+      <c r="C7" t="n">
+        <v>3520</v>
+      </c>
+      <c r="D7" t="n">
+        <v>112</v>
+      </c>
+      <c r="E7" t="n">
+        <v>814</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>2.5</v>
+        <v>25.94</v>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3138</v>
+      </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>35862</v>
+        <v>17881</v>
       </c>
       <c r="N7" t="n">
-        <v>1.18</v>
+        <v>1.34</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -822,47 +788,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C8" t="n">
-        <v>19121</v>
+        <v>19137</v>
       </c>
       <c r="D8" t="n">
-        <v>622</v>
+        <v>175</v>
       </c>
       <c r="E8" t="n">
-        <v>2091</v>
+        <v>464</v>
       </c>
       <c r="F8" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G8" t="n">
-        <v>16.08</v>
+        <v>6.81</v>
       </c>
       <c r="H8" t="n">
-        <v>4.14</v>
+        <v>15.32</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>13008</v>
+        <v>6812</v>
       </c>
       <c r="L8" t="n">
-        <v>583</v>
+        <v>111</v>
       </c>
       <c r="M8" t="n">
-        <v>354112</v>
+        <v>146703</v>
       </c>
       <c r="N8" t="n">
-        <v>7.98</v>
+        <v>7.62</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -873,47 +839,43 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44023</v>
+        <v>44021</v>
       </c>
       <c r="C9" t="n">
-        <v>27864</v>
+        <v>10679</v>
       </c>
       <c r="D9" t="n">
-        <v>319</v>
+        <v>568</v>
       </c>
       <c r="E9" t="n">
-        <v>5959</v>
+        <v>5266</v>
       </c>
       <c r="F9" t="n">
-        <v>77</v>
+        <v>421</v>
       </c>
       <c r="G9" t="n">
-        <v>24.83</v>
+        <v>49.31</v>
       </c>
       <c r="H9" t="n">
-        <v>25.84</v>
+        <v>74.12</v>
       </c>
       <c r="I9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="n">
-        <v>24000</v>
-      </c>
-      <c r="L9" t="n">
-        <v>298</v>
-      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>460970</v>
+        <v>321317</v>
       </c>
       <c r="N9" t="n">
-        <v>15.41</v>
+        <v>46.94</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -924,47 +886,47 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C10" t="n">
-        <v>19371</v>
+        <v>19121</v>
       </c>
       <c r="D10" t="n">
-        <v>422</v>
+        <v>622</v>
       </c>
       <c r="E10" t="n">
-        <v>712</v>
+        <v>2091</v>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G10" t="n">
-        <v>4.61</v>
+        <v>16.08</v>
       </c>
       <c r="H10" t="n">
-        <v>3.87</v>
+        <v>4.14</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>15451</v>
+        <v>13008</v>
       </c>
       <c r="L10" t="n">
-        <v>413</v>
+        <v>583</v>
       </c>
       <c r="M10" t="n">
-        <v>166412</v>
+        <v>354112</v>
       </c>
       <c r="N10" t="n">
-        <v>5.04</v>
+        <v>7.98</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -975,29 +937,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C11" t="n">
-        <v>69782</v>
+        <v>41571</v>
       </c>
       <c r="D11" t="n">
-        <v>1962</v>
+        <v>1499</v>
       </c>
       <c r="E11" t="n">
-        <v>10606</v>
+        <v>8571</v>
       </c>
       <c r="F11" t="n">
-        <v>456</v>
+        <v>147</v>
       </c>
       <c r="G11" t="n">
-        <v>15.2</v>
+        <v>20.62</v>
       </c>
       <c r="H11" t="n">
-        <v>23.24</v>
+        <v>9.81</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -1008,10 +970,10 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>1613285</v>
+        <v>342186</v>
       </c>
       <c r="N11" t="n">
-        <v>19.17</v>
+        <v>6.19</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1022,39 +984,47 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C12" t="n">
-        <v>14773</v>
+        <v>35679</v>
       </c>
       <c r="D12" t="n">
-        <v>543</v>
+        <v>821</v>
       </c>
       <c r="E12" t="n">
-        <v>279</v>
-      </c>
-      <c r="F12" t="inlineStr"/>
+        <v>5984</v>
+      </c>
+      <c r="F12" t="n">
+        <v>192</v>
+      </c>
       <c r="G12" t="n">
-        <v>1.89</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
+        <v>18.6</v>
+      </c>
+      <c r="H12" t="n">
+        <v>23.73</v>
+      </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>32164</v>
+      </c>
+      <c r="L12" t="n">
+        <v>809</v>
+      </c>
       <c r="M12" t="n">
-        <v>43006</v>
+        <v>368744</v>
       </c>
       <c r="N12" t="n">
-        <v>2.06</v>
+        <v>6.38</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1065,41 +1035,43 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Florida -- Miami-Dade County</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C13" t="n">
-        <v>60868</v>
+        <v>51079</v>
       </c>
       <c r="D13" t="n">
-        <v>1132</v>
+        <v>2563</v>
       </c>
       <c r="E13" t="n">
-        <v>6886</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
+        <v>6064</v>
+      </c>
+      <c r="F13" t="n">
+        <v>370</v>
+      </c>
       <c r="G13" t="n">
-        <v>20.53</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
+        <v>11.87</v>
+      </c>
+      <c r="H13" t="n">
+        <v>14.44</v>
+      </c>
       <c r="I13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="n">
-        <v>33549</v>
-      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>481976</v>
+        <v>619472</v>
       </c>
       <c r="N13" t="n">
-        <v>17.75</v>
+        <v>9.33</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1110,41 +1082,43 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Florida -- Orange County</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C14" t="n">
-        <v>16630</v>
+        <v>61006</v>
       </c>
       <c r="D14" t="n">
-        <v>80</v>
+        <v>738</v>
       </c>
       <c r="E14" t="n">
-        <v>2220</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+        <v>12323</v>
+      </c>
+      <c r="F14" t="n">
+        <v>261</v>
+      </c>
       <c r="G14" t="n">
-        <v>24.57</v>
-      </c>
-      <c r="H14" t="inlineStr"/>
+        <v>20.2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>35.37</v>
+      </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="n">
-        <v>9034</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>277193</v>
+        <v>1117489</v>
       </c>
       <c r="N14" t="n">
-        <v>20.98</v>
+        <v>16.8</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1155,47 +1129,51 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>New York -- New York</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
         <v>44023</v>
       </c>
-      <c r="C15" t="n">
-        <v>51294</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1086</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215598</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>18667</t>
+        </is>
       </c>
       <c r="E15" t="n">
-        <v>17111</v>
+        <v>33453</v>
       </c>
       <c r="F15" t="n">
-        <v>479</v>
+        <v>5225</v>
       </c>
       <c r="G15" t="n">
-        <v>45.22</v>
+        <v>30.15</v>
       </c>
       <c r="H15" t="n">
-        <v>45.84</v>
+        <v>30.52</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>37836</v>
+        <v>110942</v>
       </c>
       <c r="L15" t="n">
-        <v>1045</v>
+        <v>17118</v>
       </c>
       <c r="M15" t="n">
-        <v>1293186</v>
+        <v>2049418</v>
       </c>
       <c r="N15" t="n">
-        <v>26.58</v>
+        <v>24.27</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1206,47 +1184,49 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44022</v>
-      </c>
-      <c r="C16" t="n">
-        <v>130242</v>
-      </c>
-      <c r="D16" t="n">
-        <v>3793</v>
-      </c>
-      <c r="E16" t="n">
-        <v>3476</v>
-      </c>
-      <c r="F16" t="n">
-        <v>386</v>
+        <v>44023</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>28855</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>731</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>&lt;5</t>
+        </is>
       </c>
       <c r="G16" t="n">
-        <v>4.74</v>
-      </c>
-      <c r="H16" t="n">
-        <v>10.94</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="n">
-        <v>73398</v>
-      </c>
-      <c r="L16" t="n">
-        <v>3529</v>
-      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>823987</v>
+        <v>35862</v>
       </c>
       <c r="N16" t="n">
-        <v>8.16</v>
+        <v>1.18</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1257,47 +1237,47 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C17" t="n">
-        <v>72467</v>
+        <v>1283</v>
       </c>
       <c r="D17" t="n">
-        <v>3179</v>
+        <v>56</v>
       </c>
       <c r="E17" t="n">
-        <v>20910</v>
+        <v>138</v>
       </c>
       <c r="F17" t="n">
-        <v>1289</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>28.85</v>
+        <v>11.05</v>
       </c>
       <c r="H17" t="n">
-        <v>40.55</v>
+        <v>0</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>59766</v>
+        <v>1249</v>
       </c>
       <c r="L17" t="n">
-        <v>72448</v>
+        <v>56</v>
       </c>
       <c r="M17" t="n">
-        <v>1788090</v>
+        <v>8058</v>
       </c>
       <c r="N17" t="n">
-        <v>29.78</v>
+        <v>1.29</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1308,43 +1288,47 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mississippi</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44022</v>
+        <v>44009</v>
       </c>
       <c r="C18" t="n">
-        <v>35419</v>
+        <v>20261</v>
       </c>
       <c r="D18" t="n">
-        <v>1230</v>
+        <v>996</v>
       </c>
       <c r="E18" t="n">
-        <v>16811</v>
+        <v>5758</v>
       </c>
       <c r="F18" t="n">
-        <v>616</v>
+        <v>246</v>
       </c>
       <c r="G18" t="n">
-        <v>47.46</v>
+        <v>49.66</v>
       </c>
       <c r="H18" t="n">
-        <v>50.08</v>
+        <v>38.56</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
       </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>11594</v>
+      </c>
+      <c r="L18" t="n">
+        <v>638</v>
+      </c>
       <c r="M18" t="n">
-        <v>1125834</v>
+        <v>704896</v>
       </c>
       <c r="N18" t="n">
-        <v>37.67</v>
+        <v>11.57</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1355,81 +1339,59 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>44023</v>
-      </c>
-      <c r="C19" t="n">
-        <v>92001</v>
-      </c>
-      <c r="D19" t="n">
-        <v>6897</v>
-      </c>
-      <c r="E19" t="n">
-        <v>12624</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1426</v>
-      </c>
-      <c r="G19" t="n">
-        <v>30.31</v>
-      </c>
-      <c r="H19" t="n">
-        <v>21.68</v>
-      </c>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" t="n">
-        <v>41651</v>
-      </c>
-      <c r="L19" t="n">
-        <v>6579</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>1423319</v>
+        <v>2267875</v>
       </c>
       <c r="N19" t="n">
-        <v>11.13</v>
+        <v>5.79</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C20" t="n">
-        <v>250984</v>
+        <v>14773</v>
       </c>
       <c r="D20" t="n">
-        <v>4197</v>
+        <v>543</v>
       </c>
       <c r="E20" t="n">
-        <v>32370</v>
-      </c>
-      <c r="F20" t="n">
-        <v>821</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
-        <v>12.9</v>
-      </c>
-      <c r="H20" t="n">
-        <v>19.56</v>
-      </c>
+        <v>1.89</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="b">
         <v>1</v>
       </c>
@@ -1439,10 +1401,10 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>3316376</v>
+        <v>43006</v>
       </c>
       <c r="N20" t="n">
-        <v>16.1</v>
+        <v>2.06</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1453,39 +1415,47 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C21" t="n">
-        <v>1677</v>
+        <v>1385</v>
       </c>
       <c r="D21" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
-      </c>
-      <c r="F21" t="inlineStr"/>
+        <v>34</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
       <c r="G21" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="H21" t="inlineStr"/>
+        <v>1.43</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
       <c r="I21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
       </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+      <c r="K21" t="n">
+        <v>2376</v>
+      </c>
+      <c r="L21" t="n">
+        <v>34</v>
+      </c>
       <c r="M21" t="n">
-        <v>4630</v>
+        <v>24129</v>
       </c>
       <c r="N21" t="n">
-        <v>0.44</v>
+        <v>3.27</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1496,47 +1466,43 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Vermont</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C22" t="n">
-        <v>1283</v>
+        <v>25291</v>
       </c>
       <c r="D22" t="n">
-        <v>56</v>
+        <v>717</v>
       </c>
       <c r="E22" t="n">
-        <v>138</v>
+        <v>2887</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="G22" t="n">
-        <v>11.05</v>
+        <v>11.42</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>12.69</v>
       </c>
       <c r="I22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" t="n">
-        <v>1249</v>
-      </c>
-      <c r="L22" t="n">
-        <v>56</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>8058</v>
+        <v>3365783</v>
       </c>
       <c r="N22" t="n">
-        <v>1.29</v>
+        <v>12.07</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1547,43 +1513,47 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Connecticut</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44021</v>
+        <v>44023</v>
       </c>
       <c r="C23" t="n">
-        <v>45308</v>
+        <v>72467</v>
       </c>
       <c r="D23" t="n">
-        <v>3476</v>
+        <v>3179</v>
       </c>
       <c r="E23" t="n">
-        <v>6189</v>
+        <v>20910</v>
       </c>
       <c r="F23" t="n">
-        <v>646</v>
+        <v>1289</v>
       </c>
       <c r="G23" t="n">
-        <v>13.66</v>
+        <v>28.85</v>
       </c>
       <c r="H23" t="n">
-        <v>18.58</v>
+        <v>40.55</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
       </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
+      <c r="K23" t="n">
+        <v>59766</v>
+      </c>
+      <c r="L23" t="n">
+        <v>72448</v>
+      </c>
       <c r="M23" t="n">
-        <v>378262</v>
+        <v>1788090</v>
       </c>
       <c r="N23" t="n">
-        <v>10.56</v>
+        <v>29.78</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1594,29 +1564,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>California - San Diego</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C24" t="n">
-        <v>36591</v>
+        <v>19371</v>
       </c>
       <c r="D24" t="n">
-        <v>1725</v>
+        <v>422</v>
       </c>
       <c r="E24" t="n">
-        <v>1881</v>
+        <v>712</v>
       </c>
       <c r="F24" t="n">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="G24" t="n">
-        <v>6.34</v>
+        <v>4.61</v>
       </c>
       <c r="H24" t="n">
-        <v>7.04</v>
+        <v>3.87</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
@@ -1625,16 +1595,16 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>29686</v>
+        <v>15451</v>
       </c>
       <c r="L24" t="n">
-        <v>1662</v>
+        <v>413</v>
       </c>
       <c r="M24" t="n">
-        <v>227938</v>
+        <v>166412</v>
       </c>
       <c r="N24" t="n">
-        <v>4.12</v>
+        <v>5.04</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1645,30 +1615,26 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Florida -- Miami-Dade County</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C25" t="n">
-        <v>20998</v>
+        <v>60868</v>
       </c>
       <c r="D25" t="n">
-        <v>285</v>
+        <v>1132</v>
       </c>
       <c r="E25" t="n">
-        <v>1230</v>
-      </c>
-      <c r="F25" t="n">
-        <v>22</v>
-      </c>
+        <v>6886</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
-        <v>7.61</v>
-      </c>
-      <c r="H25" t="n">
-        <v>8.029999999999999</v>
-      </c>
+        <v>20.53</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="b">
         <v>0</v>
       </c>
@@ -1676,16 +1642,14 @@
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>16169</v>
-      </c>
-      <c r="L25" t="n">
-        <v>274</v>
-      </c>
+        <v>33549</v>
+      </c>
+      <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>90860</v>
+        <v>481976</v>
       </c>
       <c r="N25" t="n">
-        <v>4.77</v>
+        <v>17.75</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -1696,43 +1660,41 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Florida -- Orange County</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C26" t="n">
-        <v>68857</v>
+        <v>16630</v>
       </c>
       <c r="D26" t="n">
-        <v>5983</v>
+        <v>80</v>
       </c>
       <c r="E26" t="n">
-        <v>20486</v>
-      </c>
-      <c r="F26" t="n">
-        <v>2390</v>
-      </c>
+        <v>2220</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
-        <v>29.75</v>
-      </c>
-      <c r="H26" t="n">
-        <v>39.95</v>
-      </c>
+        <v>24.57</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>9034</v>
+      </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
-        <v>1375424</v>
+        <v>277193</v>
       </c>
       <c r="N26" t="n">
-        <v>13.81</v>
+        <v>20.98</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1743,76 +1705,98 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>California</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>44023</v>
+      </c>
+      <c r="C27" t="n">
+        <v>83793</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1499</v>
+      </c>
+      <c r="E27" t="n">
+        <v>13702</v>
+      </c>
+      <c r="F27" t="n">
+        <v>474</v>
+      </c>
+      <c r="G27" t="n">
+        <v>23.88</v>
+      </c>
+      <c r="H27" t="n">
+        <v>32.8</v>
+      </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>57384</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1445</v>
+      </c>
       <c r="M27" t="n">
-        <v>2267875</v>
+        <v>2179622</v>
       </c>
       <c r="N27" t="n">
-        <v>5.79</v>
+        <v>21.46</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>California - Los Angeles</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44023</v>
+        <v>44022</v>
       </c>
       <c r="C28" t="n">
-        <v>51079</v>
+        <v>130242</v>
       </c>
       <c r="D28" t="n">
-        <v>2563</v>
+        <v>3793</v>
       </c>
       <c r="E28" t="n">
-        <v>6064</v>
+        <v>3476</v>
       </c>
       <c r="F28" t="n">
-        <v>370</v>
+        <v>386</v>
       </c>
       <c r="G28" t="n">
-        <v>11.87</v>
+        <v>4.74</v>
       </c>
       <c r="H28" t="n">
-        <v>14.44</v>
+        <v>10.94</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>73398</v>
+      </c>
+      <c r="L28" t="n">
+        <v>3529</v>
+      </c>
       <c r="M28" t="n">
-        <v>619472</v>
+        <v>823987</v>
       </c>
       <c r="N28" t="n">
-        <v>9.33</v>
+        <v>8.16</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1823,47 +1807,39 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C29" t="n">
-        <v>1385</v>
+        <v>1677</v>
       </c>
       <c r="D29" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E29" t="n">
-        <v>34</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0</v>
-      </c>
+        <v>0.42</v>
+      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="b">
         <v>1</v>
       </c>
-      <c r="K29" t="n">
-        <v>2376</v>
-      </c>
-      <c r="L29" t="n">
-        <v>34</v>
-      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>24129</v>
+        <v>4630</v>
       </c>
       <c r="N29" t="n">
-        <v>3.27</v>
+        <v>0.44</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1874,47 +1850,43 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44023</v>
+        <v>44021</v>
       </c>
       <c r="C30" t="n">
-        <v>35679</v>
+        <v>45308</v>
       </c>
       <c r="D30" t="n">
-        <v>821</v>
+        <v>3476</v>
       </c>
       <c r="E30" t="n">
-        <v>5984</v>
+        <v>6189</v>
       </c>
       <c r="F30" t="n">
-        <v>192</v>
+        <v>646</v>
       </c>
       <c r="G30" t="n">
-        <v>18.6</v>
+        <v>13.66</v>
       </c>
       <c r="H30" t="n">
-        <v>23.73</v>
+        <v>18.58</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" t="n">
-        <v>32164</v>
-      </c>
-      <c r="L30" t="n">
-        <v>809</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
-        <v>368744</v>
+        <v>378262</v>
       </c>
       <c r="N30" t="n">
-        <v>6.38</v>
+        <v>10.56</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1925,29 +1897,29 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C31" t="n">
-        <v>114401</v>
+        <v>69782</v>
       </c>
       <c r="D31" t="n">
-        <v>2996</v>
+        <v>1962</v>
       </c>
       <c r="E31" t="n">
-        <v>31052</v>
+        <v>10606</v>
       </c>
       <c r="F31" t="n">
-        <v>1397</v>
+        <v>456</v>
       </c>
       <c r="G31" t="n">
-        <v>27.14</v>
+        <v>15.2</v>
       </c>
       <c r="H31" t="n">
-        <v>46.63</v>
+        <v>23.24</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -1958,10 +1930,10 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="n">
-        <v>3239300</v>
+        <v>1613285</v>
       </c>
       <c r="N31" t="n">
-        <v>31.46</v>
+        <v>19.17</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -1972,29 +1944,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44022</v>
+        <v>44015</v>
       </c>
       <c r="C32" t="n">
-        <v>39218</v>
+        <v>16491</v>
       </c>
       <c r="D32" t="n">
-        <v>1424</v>
+        <v>960</v>
       </c>
       <c r="E32" t="n">
-        <v>1520</v>
+        <v>1592</v>
       </c>
       <c r="F32" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G32" t="n">
-        <v>5.43</v>
+        <v>12.29</v>
       </c>
       <c r="H32" t="n">
-        <v>3.39</v>
+        <v>6.14</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -2003,16 +1975,16 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>27979</v>
+        <v>12950</v>
       </c>
       <c r="L32" t="n">
-        <v>1355</v>
+        <v>782</v>
       </c>
       <c r="M32" t="n">
-        <v>269854</v>
+        <v>69254</v>
       </c>
       <c r="N32" t="n">
-        <v>3.7</v>
+        <v>6.55</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2023,43 +1995,47 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44021</v>
+        <v>44023</v>
       </c>
       <c r="C33" t="n">
-        <v>10679</v>
+        <v>20998</v>
       </c>
       <c r="D33" t="n">
-        <v>568</v>
+        <v>285</v>
       </c>
       <c r="E33" t="n">
-        <v>5266</v>
+        <v>1230</v>
       </c>
       <c r="F33" t="n">
-        <v>421</v>
+        <v>22</v>
       </c>
       <c r="G33" t="n">
-        <v>49.31</v>
+        <v>7.61</v>
       </c>
       <c r="H33" t="n">
-        <v>74.12</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="I33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="b">
         <v>1</v>
       </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
+      <c r="K33" t="n">
+        <v>16169</v>
+      </c>
+      <c r="L33" t="n">
+        <v>274</v>
+      </c>
       <c r="M33" t="n">
-        <v>321317</v>
+        <v>90860</v>
       </c>
       <c r="N33" t="n">
-        <v>46.94</v>
+        <v>4.77</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2070,43 +2046,43 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C34" t="n">
-        <v>12743</v>
+        <v>114401</v>
       </c>
       <c r="D34" t="n">
-        <v>106</v>
+        <v>2996</v>
       </c>
       <c r="E34" t="n">
-        <v>3254</v>
+        <v>31052</v>
       </c>
       <c r="F34" t="n">
-        <v>132</v>
+        <v>1397</v>
       </c>
       <c r="G34" t="n">
-        <v>25.54</v>
+        <v>27.14</v>
       </c>
       <c r="H34" t="n">
-        <v>124.53</v>
+        <v>46.63</v>
       </c>
       <c r="I34" t="b">
         <v>1</v>
       </c>
       <c r="J34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>209892</v>
+        <v>3239300</v>
       </c>
       <c r="N34" t="n">
-        <v>22.11</v>
+        <v>31.46</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2117,41 +2093,47 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44023</v>
+        <v>44022</v>
       </c>
       <c r="C35" t="n">
-        <v>3520</v>
+        <v>13430</v>
       </c>
       <c r="D35" t="n">
-        <v>112</v>
+        <v>359</v>
       </c>
       <c r="E35" t="n">
-        <v>814</v>
-      </c>
-      <c r="F35" t="inlineStr"/>
+        <v>3889</v>
+      </c>
+      <c r="F35" t="n">
+        <v>145</v>
+      </c>
       <c r="G35" t="n">
-        <v>25.94</v>
-      </c>
-      <c r="H35" t="inlineStr"/>
+        <v>31.17</v>
+      </c>
+      <c r="H35" t="n">
+        <v>40.39</v>
+      </c>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>3138</v>
-      </c>
-      <c r="L35" t="inlineStr"/>
+        <v>12475</v>
+      </c>
+      <c r="L35" t="n">
+        <v>359</v>
+      </c>
       <c r="M35" t="n">
-        <v>17881</v>
+        <v>252321</v>
       </c>
       <c r="N35" t="n">
-        <v>1.34</v>
+        <v>26.44</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2162,32 +2144,32 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C36" t="n">
-        <v>34658</v>
+        <v>10505</v>
       </c>
       <c r="D36" t="n">
-        <v>748</v>
+        <v>101</v>
       </c>
       <c r="E36" t="n">
-        <v>3011</v>
+        <v>149</v>
       </c>
       <c r="F36" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>8.69</v>
+        <v>1.42</v>
       </c>
       <c r="H36" t="n">
-        <v>4.81</v>
+        <v>0.99</v>
       </c>
       <c r="I36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>
@@ -2195,10 +2177,10 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
-        <v>109911</v>
+        <v>11536</v>
       </c>
       <c r="N36" t="n">
-        <v>3.51</v>
+        <v>0.68</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2209,29 +2191,29 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C37" t="n">
-        <v>83793</v>
+        <v>92001</v>
       </c>
       <c r="D37" t="n">
-        <v>1499</v>
+        <v>6897</v>
       </c>
       <c r="E37" t="n">
-        <v>13702</v>
+        <v>12624</v>
       </c>
       <c r="F37" t="n">
-        <v>474</v>
+        <v>1426</v>
       </c>
       <c r="G37" t="n">
-        <v>23.88</v>
+        <v>30.31</v>
       </c>
       <c r="H37" t="n">
-        <v>32.8</v>
+        <v>21.68</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -2240,16 +2222,16 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>57384</v>
+        <v>41651</v>
       </c>
       <c r="L37" t="n">
-        <v>1445</v>
+        <v>6579</v>
       </c>
       <c r="M37" t="n">
-        <v>2179622</v>
+        <v>1423319</v>
       </c>
       <c r="N37" t="n">
-        <v>21.46</v>
+        <v>11.13</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2260,43 +2242,47 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C38" t="n">
-        <v>152962</v>
+        <v>36591</v>
       </c>
       <c r="D38" t="n">
-        <v>7168</v>
+        <v>1725</v>
       </c>
       <c r="E38" t="n">
-        <v>25689</v>
+        <v>1881</v>
       </c>
       <c r="F38" t="n">
-        <v>1982</v>
+        <v>117</v>
       </c>
       <c r="G38" t="n">
-        <v>16.79</v>
+        <v>6.34</v>
       </c>
       <c r="H38" t="n">
-        <v>27.65</v>
+        <v>7.04</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
       </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
+      <c r="K38" t="n">
+        <v>29686</v>
+      </c>
+      <c r="L38" t="n">
+        <v>1662</v>
+      </c>
       <c r="M38" t="n">
-        <v>1824125</v>
+        <v>227938</v>
       </c>
       <c r="N38" t="n">
-        <v>14.23</v>
+        <v>4.12</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2307,43 +2293,47 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Idaho</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44023</v>
+        <v>44022</v>
       </c>
       <c r="C39" t="n">
-        <v>10505</v>
+        <v>39218</v>
       </c>
       <c r="D39" t="n">
-        <v>101</v>
+        <v>1424</v>
       </c>
       <c r="E39" t="n">
-        <v>149</v>
+        <v>1520</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="G39" t="n">
-        <v>1.42</v>
+        <v>5.43</v>
       </c>
       <c r="H39" t="n">
-        <v>0.99</v>
+        <v>3.39</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>27979</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1355</v>
+      </c>
       <c r="M39" t="n">
-        <v>11536</v>
+        <v>269854</v>
       </c>
       <c r="N39" t="n">
-        <v>0.68</v>
+        <v>3.7</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -2354,43 +2344,43 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C40" t="n">
-        <v>41571</v>
+        <v>250984</v>
       </c>
       <c r="D40" t="n">
-        <v>1499</v>
+        <v>4197</v>
       </c>
       <c r="E40" t="n">
-        <v>8571</v>
+        <v>32370</v>
       </c>
       <c r="F40" t="n">
-        <v>147</v>
+        <v>821</v>
       </c>
       <c r="G40" t="n">
-        <v>20.62</v>
+        <v>12.9</v>
       </c>
       <c r="H40" t="n">
-        <v>9.81</v>
+        <v>19.56</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="n">
-        <v>342186</v>
+        <v>3316376</v>
       </c>
       <c r="N40" t="n">
-        <v>6.19</v>
+        <v>16.1</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2401,29 +2391,29 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
         <v>44023</v>
       </c>
       <c r="C41" t="n">
-        <v>111398</v>
+        <v>68857</v>
       </c>
       <c r="D41" t="n">
-        <v>8310</v>
+        <v>5983</v>
       </c>
       <c r="E41" t="n">
-        <v>10477</v>
+        <v>20486</v>
       </c>
       <c r="F41" t="n">
-        <v>684</v>
+        <v>2390</v>
       </c>
       <c r="G41" t="n">
-        <v>9.41</v>
+        <v>29.75</v>
       </c>
       <c r="H41" t="n">
-        <v>8.23</v>
+        <v>39.95</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
@@ -2434,10 +2424,10 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="n">
-        <v>510558</v>
+        <v>1375424</v>
       </c>
       <c r="N41" t="n">
-        <v>7.48</v>
+        <v>13.81</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -2448,47 +2438,43 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
         <v>44022</v>
       </c>
       <c r="C42" t="n">
-        <v>13430</v>
+        <v>35419</v>
       </c>
       <c r="D42" t="n">
-        <v>359</v>
+        <v>1230</v>
       </c>
       <c r="E42" t="n">
-        <v>3889</v>
+        <v>16811</v>
       </c>
       <c r="F42" t="n">
-        <v>145</v>
+        <v>616</v>
       </c>
       <c r="G42" t="n">
-        <v>31.17</v>
+        <v>47.46</v>
       </c>
       <c r="H42" t="n">
-        <v>40.39</v>
+        <v>50.08</v>
       </c>
       <c r="I42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="b">
-        <v>0</v>
-      </c>
-      <c r="K42" t="n">
-        <v>12475</v>
-      </c>
-      <c r="L42" t="n">
-        <v>359</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
       <c r="M42" t="n">
-        <v>252321</v>
+        <v>1125834</v>
       </c>
       <c r="N42" t="n">
-        <v>26.44</v>
+        <v>37.67</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -2499,47 +2485,43 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44009</v>
+        <v>44023</v>
       </c>
       <c r="C43" t="n">
-        <v>20261</v>
+        <v>12743</v>
       </c>
       <c r="D43" t="n">
-        <v>996</v>
+        <v>106</v>
       </c>
       <c r="E43" t="n">
-        <v>5758</v>
+        <v>3254</v>
       </c>
       <c r="F43" t="n">
-        <v>246</v>
+        <v>132</v>
       </c>
       <c r="G43" t="n">
-        <v>49.66</v>
+        <v>25.54</v>
       </c>
       <c r="H43" t="n">
-        <v>38.56</v>
+        <v>124.53</v>
       </c>
       <c r="I43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="b">
-        <v>1</v>
-      </c>
-      <c r="K43" t="n">
-        <v>11594</v>
-      </c>
-      <c r="L43" t="n">
-        <v>638</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
       <c r="M43" t="n">
-        <v>704896</v>
+        <v>209892</v>
       </c>
       <c r="N43" t="n">
-        <v>11.57</v>
+        <v>22.11</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>

</xml_diff>